<commit_message>
update spreadsheet and changed to use media eleme
media element allows for pausing which is good for long sounds...but now
the back button does not work because I believe the begin invoke.
</commit_message>
<xml_diff>
--- a/Baby App Pics and Sounds.xlsx
+++ b/Baby App Pics and Sounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tedyoung\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-hub\BabyApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="94">
   <si>
     <t xml:space="preserve">        Animals.Add(new Box("Anteater", "/Assets/Pics/Animals/anteater80x100.png", "/Assets/Pics/Animals/anteater480x800.png", "/Assets/Sounds/Animals/anteater.wav"));</t>
   </si>
@@ -209,9 +209,6 @@
     <t xml:space="preserve">            Animals.Add(new Box("Wolf", "/Assets/Pics/Animals/wolf80x100.png", "/Assets/Pics/Animals/wolf480x800.png", "/Assets/Sounds/Animals/wolf.wav"));</t>
   </si>
   <si>
-    <t xml:space="preserve">            Animals.Add(new Box("", "", "", ""));</t>
-  </si>
-  <si>
     <t>Pic</t>
   </si>
   <si>
@@ -258,6 +255,57 @@
   </si>
   <si>
     <t>rooster</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>not working</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>text does not display, sounds is wrong</t>
+  </si>
+  <si>
+    <t>sound is wrong</t>
+  </si>
+  <si>
+    <t>not great sound</t>
+  </si>
+  <si>
+    <t>voice says name wrong</t>
+  </si>
+  <si>
+    <t>pic not great as portrait</t>
+  </si>
+  <si>
+    <t>quick sound</t>
+  </si>
+  <si>
+    <t>way too quick and not sure what it is a sound of</t>
+  </si>
+  <si>
+    <t>a little short</t>
+  </si>
+  <si>
+    <t>wrong sound</t>
+  </si>
+  <si>
+    <t>too short</t>
+  </si>
+  <si>
+    <t>text does not display, sounds is maybe wrong not sure</t>
+  </si>
+  <si>
+    <t>not sure it is right sound</t>
+  </si>
+  <si>
+    <t>a bit short</t>
+  </si>
+  <si>
+    <t>way too quick</t>
   </si>
 </sst>
 </file>
@@ -578,439 +626,643 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C77"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="167.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="167.86328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C20" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C23" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C32" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C33" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C34" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C36" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C37" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B40" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C42" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C43" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B51" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B52" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C45" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C46" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C47" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C48" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B49" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C50" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C51" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B52" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C53" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C55" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C56" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B57" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" t="s">
+        <v>91</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B58" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B59" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C58" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C59" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C62" s="1" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B61" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B62" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C65" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C66" s="1" t="s">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B65" t="s">
+        <v>77</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C67" s="1" t="s">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C68" s="1" t="s">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B67" t="s">
+        <v>77</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C69" s="1" t="s">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C70" s="1" t="s">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B69" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69" t="s">
+        <v>93</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C71" s="1" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B70" t="s">
+        <v>77</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C72" s="1" t="s">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B71" t="s">
+        <v>77</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C73" s="1" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B72" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" t="s">
+        <v>91</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C74" s="1" t="s">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B73" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" t="s">
+        <v>91</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C75" s="1" t="s">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B74" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C76" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C77" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>